<commit_message>
Added Station to nested PERMANOVA, and final table
</commit_message>
<xml_diff>
--- a/analysis/permanova_results.xlsx
+++ b/analysis/permanova_results.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="0" windowWidth="23980" windowHeight="14240" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14280" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Overall" sheetId="1" r:id="rId1"/>
     <sheet name="Ver_Lake" sheetId="2" r:id="rId2"/>
     <sheet name="BCC_Lake" sheetId="3" r:id="rId3"/>
+    <sheet name="Final Table" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="33">
   <si>
     <t>Depth</t>
   </si>
@@ -109,11 +110,26 @@
   <si>
     <t>Lake_Type</t>
   </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Station</t>
+  </si>
+  <si>
+    <t>Verrucomicrobia</t>
+  </si>
+  <si>
+    <t>Whole Community</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -177,7 +193,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -244,8 +260,47 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="89">
+  <cellStyleXfs count="159">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -335,8 +390,78 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -354,8 +479,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="89">
+  <cellStyles count="159">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -400,6 +541,41 @@
     <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -444,6 +620,41 @@
     <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -775,8 +986,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1660,34 +1871,34 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R28"/>
+  <dimension ref="A1:T31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N15" sqref="N15:N16"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="12.1640625" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" customWidth="1"/>
-    <col min="14" max="14" width="12.6640625" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" customWidth="1"/>
+    <col min="16" max="16" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="25">
+    <row r="1" spans="1:20" ht="25">
       <c r="A1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>26</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:20">
       <c r="C2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1697,29 +1908,35 @@
       <c r="E2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="F2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="K2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="L2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="M2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="N2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="R2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="S2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="T2" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:20">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -1735,14 +1952,14 @@
       <c r="E3" s="5">
         <v>1E-3</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="F3" s="14">
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="I3" s="5">
-        <v>1E-3</v>
+      <c r="I3" s="4" t="s">
+        <v>3</v>
       </c>
       <c r="J3" s="5">
         <v>1E-3</v>
@@ -1753,23 +1970,29 @@
       <c r="L3" s="5">
         <v>1E-3</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="M3" s="5">
+        <v>1E-3</v>
+      </c>
+      <c r="N3" s="14">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="P3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="O3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="P3" s="5">
+      <c r="Q3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="R3" s="5">
         <v>2E-3</v>
       </c>
-      <c r="Q3" s="5">
-        <v>1E-3</v>
-      </c>
-      <c r="R3" s="5">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18">
+      <c r="S3" s="5">
+        <v>1E-3</v>
+      </c>
+      <c r="T3" s="5">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20">
       <c r="A4" s="2"/>
       <c r="B4" s="4" t="s">
         <v>4</v>
@@ -1783,37 +2006,43 @@
       <c r="E4" s="5">
         <v>0.43081999999999998</v>
       </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="4" t="s">
+      <c r="F4" s="14">
+        <v>3.2439999999999997E-2</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="5">
+      <c r="J4" s="5">
         <v>0.30093999999999999</v>
       </c>
-      <c r="J4" s="5">
+      <c r="K4" s="5">
         <v>0.28632999999999997</v>
       </c>
-      <c r="K4" s="5">
+      <c r="L4" s="5">
         <v>0.41320000000000001</v>
       </c>
-      <c r="L4" s="5">
+      <c r="M4" s="5">
         <v>0.21914</v>
       </c>
-      <c r="N4" s="2"/>
-      <c r="O4" s="4" t="s">
+      <c r="N4" s="14">
+        <v>9.3340000000000006E-2</v>
+      </c>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="P4" s="5">
+      <c r="R4" s="5">
         <v>3.5479999999999998E-2</v>
       </c>
-      <c r="Q4" s="5">
+      <c r="S4" s="5">
         <v>0.11226</v>
       </c>
-      <c r="R4" s="5">
-        <v>0.77229999999999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18">
+      <c r="T4" s="5">
+        <v>7.7229999999999993E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -1829,41 +2058,47 @@
       <c r="E5" s="5">
         <v>1E-3</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="F5" s="14">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="I5" s="5">
+      <c r="I5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J5" s="5">
         <v>1.9E-2</v>
       </c>
-      <c r="J5" s="5">
+      <c r="K5" s="5">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="K5" s="5">
+      <c r="L5" s="5">
         <v>8.5999999999999993E-2</v>
       </c>
-      <c r="L5" s="5">
+      <c r="M5" s="5">
         <v>0.75600000000000001</v>
       </c>
-      <c r="N5" s="1" t="s">
+      <c r="N5" s="14">
+        <v>0.41599999999999998</v>
+      </c>
+      <c r="P5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="O5" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="P5" s="5">
+      <c r="Q5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="R5" s="5">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="Q5" s="5">
+      <c r="S5" s="5">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="R5" s="5">
+      <c r="T5" s="5">
         <v>2E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:20">
       <c r="A6" s="3"/>
       <c r="B6" s="4" t="s">
         <v>7</v>
@@ -1877,48 +2112,54 @@
       <c r="E6" s="5">
         <v>11.22</v>
       </c>
-      <c r="G6" s="3"/>
-      <c r="H6" s="4" t="s">
+      <c r="F6" s="5">
+        <v>8.5780969999999996</v>
+      </c>
+      <c r="H6" s="3"/>
+      <c r="I6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="5">
+      <c r="J6" s="5">
         <v>4.0681330000000004</v>
       </c>
-      <c r="J6" s="5">
+      <c r="K6" s="5">
         <v>9.3926859999999994</v>
       </c>
-      <c r="K6" s="5">
+      <c r="L6" s="5">
         <v>2.717009</v>
       </c>
-      <c r="L6" s="5">
+      <c r="M6" s="5">
         <v>0.29795260000000001</v>
       </c>
-      <c r="N6" s="3"/>
-      <c r="O6" s="4" t="s">
+      <c r="N6" s="5">
+        <v>0.96834659999999995</v>
+      </c>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="P6" s="5">
+      <c r="R6" s="5">
         <v>9.5348129999999998</v>
       </c>
-      <c r="Q6" s="5">
+      <c r="S6" s="5">
         <v>8.0830979999999997</v>
       </c>
-      <c r="R6" s="5">
+      <c r="T6" s="5">
         <v>8.0387830000000005</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
-      <c r="I8" s="4" t="s">
+    <row r="8" spans="1:20">
+      <c r="J8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="4" t="s">
+      <c r="K8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="K8" s="4" t="s">
+      <c r="L8" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:20">
       <c r="C9" s="4" t="s">
         <v>19</v>
       </c>
@@ -1928,32 +2169,33 @@
       <c r="E9" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="F9" s="16"/>
+      <c r="H9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H9" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="I9" s="5">
+      <c r="I9" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="J9" s="5">
         <v>0.313</v>
       </c>
-      <c r="J9" s="5">
-        <v>1E-3</v>
-      </c>
       <c r="K9" s="5">
         <v>1E-3</v>
       </c>
-      <c r="P9" s="4" t="s">
+      <c r="L9" s="5">
+        <v>1E-3</v>
+      </c>
+      <c r="R9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="Q9" s="4" t="s">
+      <c r="S9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="R9" s="4" t="s">
+      <c r="T9" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:20">
       <c r="A10" s="7" t="s">
         <v>5</v>
       </c>
@@ -1969,36 +2211,37 @@
       <c r="E10" s="5">
         <v>1E-3</v>
       </c>
-      <c r="G10" s="2"/>
-      <c r="H10" s="12" t="s">
+      <c r="F10" s="15"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="I10" s="5">
+      <c r="J10" s="5">
         <v>2.24E-2</v>
       </c>
-      <c r="J10" s="5">
+      <c r="K10" s="5">
         <v>0.39374999999999999</v>
       </c>
-      <c r="K10" s="5">
+      <c r="L10" s="5">
         <v>0.39372000000000001</v>
       </c>
-      <c r="N10" s="7" t="s">
+      <c r="P10" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="O10" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="P10" s="5">
-        <v>1E-3</v>
-      </c>
-      <c r="Q10" s="5">
-        <v>1E-3</v>
+      <c r="Q10" s="13" t="s">
+        <v>3</v>
       </c>
       <c r="R10" s="5">
+        <v>1E-3</v>
+      </c>
+      <c r="S10" s="5">
+        <v>1E-3</v>
+      </c>
+      <c r="T10" s="5">
         <v>1.9E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:20">
       <c r="A11" s="8"/>
       <c r="B11" s="8" t="s">
         <v>4</v>
@@ -2012,36 +2255,37 @@
       <c r="E11" s="5">
         <v>0.18953</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="F11" s="15"/>
+      <c r="H11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H11" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="I11" s="5">
+      <c r="I11" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="J11" s="5">
         <v>0.81100000000000005</v>
       </c>
-      <c r="J11" s="5">
+      <c r="K11" s="5">
         <v>1.6E-2</v>
       </c>
-      <c r="K11" s="5">
+      <c r="L11" s="5">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="N11" s="8"/>
-      <c r="O11" s="8" t="s">
+      <c r="P11" s="8"/>
+      <c r="Q11" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="P11" s="5">
+      <c r="R11" s="5">
         <v>6.701E-2</v>
       </c>
-      <c r="Q11" s="5">
+      <c r="S11" s="5">
         <v>0.17293</v>
       </c>
-      <c r="R11" s="5">
+      <c r="T11" s="5">
         <v>2.92E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:20">
       <c r="A12" s="9" t="s">
         <v>6</v>
       </c>
@@ -2057,36 +2301,37 @@
       <c r="E12" s="5">
         <v>0.82499999999999996</v>
       </c>
-      <c r="G12" s="3"/>
-      <c r="H12" s="12" t="s">
+      <c r="F12" s="15"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="I12" s="5">
+      <c r="J12" s="5">
         <v>5.3591560000000003E-2</v>
       </c>
-      <c r="J12" s="5">
+      <c r="K12" s="5">
         <v>6.5365489999999999</v>
       </c>
-      <c r="K12" s="5">
+      <c r="L12" s="5">
         <v>8.6685370000000006</v>
       </c>
-      <c r="N12" s="9" t="s">
+      <c r="P12" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="O12" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="P12" s="5">
-        <v>1E-3</v>
-      </c>
-      <c r="Q12" s="5">
+      <c r="Q12" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="R12" s="5">
+        <v>1E-3</v>
+      </c>
+      <c r="S12" s="5">
         <v>0.42</v>
       </c>
-      <c r="R12" s="5">
+      <c r="T12" s="5">
         <v>4.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:20">
       <c r="A13" s="10"/>
       <c r="B13" s="8" t="s">
         <v>7</v>
@@ -2100,283 +2345,347 @@
       <c r="E13" s="5">
         <v>4.6941709999999998E-2</v>
       </c>
-      <c r="N13" s="10"/>
-      <c r="O13" s="8" t="s">
+      <c r="F13" s="15"/>
+      <c r="P13" s="10"/>
+      <c r="Q13" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="P13" s="5">
+      <c r="R13" s="5">
         <v>16.4969</v>
       </c>
-      <c r="Q13" s="5">
+      <c r="S13" s="5">
         <v>0.72478569999999998</v>
       </c>
-      <c r="R13" s="5">
+      <c r="T13" s="5">
         <v>4.1811259999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:18">
-      <c r="I14" s="4" t="s">
+    <row r="14" spans="1:20">
+      <c r="J14" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="J14" s="4" t="s">
+      <c r="K14" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="K14" s="4" t="s">
+      <c r="L14" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:20">
       <c r="A15" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B15" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="H15" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I15" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="J15" s="5">
+        <v>1E-3</v>
+      </c>
+      <c r="K15" s="5">
+        <v>1E-3</v>
+      </c>
+      <c r="L15" s="5">
+        <v>1E-3</v>
+      </c>
+      <c r="P15" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q15" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="R15" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="S15" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G15" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="H15" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="I15" s="5">
-        <v>1E-3</v>
-      </c>
-      <c r="J15" s="5">
-        <v>1E-3</v>
-      </c>
-      <c r="K15" s="5">
-        <v>1E-3</v>
-      </c>
-      <c r="N15" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="O15" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="P15" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q15" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18">
+    </row>
+    <row r="16" spans="1:20">
       <c r="A16" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B16" s="5">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="C16" s="5">
-        <v>1E-3</v>
-      </c>
-      <c r="D16" s="5">
-        <v>1E-3</v>
-      </c>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8" t="s">
+        <v>1E-3</v>
+      </c>
+      <c r="C16" s="19">
+        <v>1E-3</v>
+      </c>
+      <c r="D16" s="19">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="E16" s="19">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="I16" s="5">
+      <c r="J16" s="5">
         <v>0.19445999999999999</v>
       </c>
-      <c r="J16" s="5">
+      <c r="K16" s="5">
         <v>0.39180999999999999</v>
       </c>
-      <c r="K16" s="5">
+      <c r="L16" s="5">
         <v>0.51146000000000003</v>
       </c>
-      <c r="N16" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="O16" s="5">
-        <v>1E-3</v>
-      </c>
-      <c r="P16" s="5">
-        <v>1E-3</v>
+      <c r="P16" s="4" t="s">
+        <v>3</v>
       </c>
       <c r="Q16" s="5">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="17" spans="1:17">
+      <c r="R16" s="5">
+        <v>1E-3</v>
+      </c>
+      <c r="S16" s="5">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19">
       <c r="A17" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="5">
-        <v>4.616E-2</v>
-      </c>
-      <c r="C17" s="5">
-        <v>0.17534</v>
-      </c>
-      <c r="D17" s="14">
-        <v>0.43081999999999998</v>
-      </c>
-      <c r="G17" s="9" t="s">
+      <c r="B17" s="19">
+        <v>0.17341000000000001</v>
+      </c>
+      <c r="C17" s="19">
+        <v>0.43275000000000002</v>
+      </c>
+      <c r="D17" s="19">
+        <v>3.4549999999999997E-2</v>
+      </c>
+      <c r="E17" s="19">
+        <v>4.5089999999999998E-2</v>
+      </c>
+      <c r="H17" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H17" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="I17" s="5">
+      <c r="I17" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="J17" s="5">
         <v>0.14099999999999999</v>
       </c>
-      <c r="J17" s="5">
+      <c r="K17" s="5">
         <v>7.5999999999999998E-2</v>
       </c>
-      <c r="K17" s="5">
+      <c r="L17" s="5">
         <v>0.23499999999999999</v>
       </c>
-      <c r="N17" s="4" t="s">
+      <c r="P17" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="O17" s="5">
+      <c r="Q17" s="5">
         <v>3.5319999999999997E-2</v>
       </c>
-      <c r="P17" s="14">
+      <c r="R17" s="14">
         <v>0.11226</v>
       </c>
-      <c r="Q17" s="14">
+      <c r="S17" s="14">
         <v>7.7229999999999993E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:17">
-      <c r="G18" s="10"/>
-      <c r="H18" s="8" t="s">
+    <row r="18" spans="1:19">
+      <c r="H18" s="10"/>
+      <c r="I18" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I18" s="5">
+      <c r="J18" s="5">
         <v>2.4310740000000002</v>
       </c>
-      <c r="J18" s="5">
+      <c r="K18" s="5">
         <v>3.423727</v>
       </c>
-      <c r="K18" s="5">
+      <c r="L18" s="5">
         <v>1.4319219999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:17">
-      <c r="I20" s="4" t="s">
+    <row r="19" spans="1:19">
+      <c r="B19" s="15"/>
+    </row>
+    <row r="20" spans="1:19">
+      <c r="B20" s="16"/>
+      <c r="E20" s="15"/>
+      <c r="J20" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="J20" s="4" t="s">
+      <c r="K20" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="K20" s="4" t="s">
+      <c r="L20" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:17">
-      <c r="G21" s="7" t="s">
+    <row r="21" spans="1:19">
+      <c r="B21" s="15"/>
+      <c r="E21" s="24"/>
+      <c r="H21" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H21" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="I21" s="5">
-        <v>1E-3</v>
+      <c r="I21" s="13" t="s">
+        <v>3</v>
       </c>
       <c r="J21" s="5">
         <v>1E-3</v>
       </c>
       <c r="K21" s="5">
+        <v>1E-3</v>
+      </c>
+      <c r="L21" s="5">
         <v>2.5999999999999999E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:17">
-      <c r="G22" s="8"/>
-      <c r="H22" s="8" t="s">
+    <row r="22" spans="1:19">
+      <c r="B22" s="15"/>
+      <c r="E22" s="24"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="I22" s="5">
+      <c r="J22" s="5">
         <v>0.21356</v>
       </c>
-      <c r="J22" s="5">
+      <c r="K22" s="5">
         <v>0.25880999999999998</v>
       </c>
-      <c r="K22" s="5">
+      <c r="L22" s="5">
         <v>5.5530000000000003E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:17">
-      <c r="G23" s="9" t="s">
+    <row r="23" spans="1:19">
+      <c r="B23" s="24"/>
+      <c r="E23" s="24"/>
+      <c r="H23" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H23" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="I23" s="5">
+      <c r="I23" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="J23" s="5">
         <v>0.81399999999999995</v>
       </c>
-      <c r="J23" s="5">
+      <c r="K23" s="5">
         <v>0.47199999999999998</v>
       </c>
-      <c r="K23" s="5">
+      <c r="L23" s="5">
         <v>0.58799999999999997</v>
       </c>
     </row>
-    <row r="24" spans="1:17">
-      <c r="G24" s="10"/>
-      <c r="H24" s="8" t="s">
+    <row r="24" spans="1:19">
+      <c r="B24" s="24"/>
+      <c r="E24" s="24"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I24" s="5">
+      <c r="J24" s="5">
         <v>5.5722130000000002E-2</v>
       </c>
-      <c r="J24" s="5">
+      <c r="K24" s="5">
         <v>0.50645459999999998</v>
       </c>
-      <c r="K24" s="5">
+      <c r="L24" s="5">
         <v>0.29260639999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:17">
-      <c r="G26" s="4" t="s">
+    <row r="25" spans="1:19">
+      <c r="B25" s="24"/>
+      <c r="E25" s="24"/>
+    </row>
+    <row r="26" spans="1:19">
+      <c r="B26" s="24"/>
+      <c r="E26" s="24"/>
+      <c r="H26" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H26" s="11" t="s">
+      <c r="I26" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="J26" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="K26" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="L26" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="M26" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="I26" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="J26" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17">
-      <c r="G27" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="H27" s="5">
-        <v>1E-3</v>
-      </c>
-      <c r="I27" s="5">
-        <v>1E-3</v>
-      </c>
-      <c r="J27" s="5">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17">
-      <c r="G28" s="4" t="s">
+    </row>
+    <row r="27" spans="1:19">
+      <c r="B27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="H27" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I27" s="19">
+        <v>1E-3</v>
+      </c>
+      <c r="J27" s="19">
+        <v>1E-3</v>
+      </c>
+      <c r="K27" s="19">
+        <v>1E-3</v>
+      </c>
+      <c r="L27" s="19">
+        <v>1E-3</v>
+      </c>
+      <c r="M27" s="19">
+        <v>3.5999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19">
+      <c r="B28" s="24"/>
+      <c r="E28" s="24"/>
+      <c r="H28" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H28" s="5">
-        <v>0.30093999999999999</v>
-      </c>
-      <c r="I28" s="14">
-        <v>0.21645</v>
-      </c>
-      <c r="J28" s="14">
+      <c r="I28" s="19">
+        <v>0.28632999999999997</v>
+      </c>
+      <c r="J28" s="19">
         <v>0.12687000000000001</v>
       </c>
+      <c r="K28" s="19">
+        <v>0.21772</v>
+      </c>
+      <c r="L28" s="19">
+        <v>6.93E-2</v>
+      </c>
+      <c r="M28" s="19">
+        <v>1.2869999999999999E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19">
+      <c r="B29" s="24"/>
+      <c r="E29" s="24"/>
+    </row>
+    <row r="30" spans="1:19">
+      <c r="B30" s="24"/>
+      <c r="E30" s="24"/>
+      <c r="H30" s="17"/>
+    </row>
+    <row r="31" spans="1:19">
+      <c r="B31" s="15"/>
+      <c r="E31" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2391,34 +2700,34 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R28"/>
+  <dimension ref="A1:T31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N15" sqref="N15:N16"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="12.6640625" customWidth="1"/>
-    <col min="7" max="7" width="12.5" customWidth="1"/>
-    <col min="14" max="14" width="12.83203125" customWidth="1"/>
+    <col min="8" max="8" width="12.5" customWidth="1"/>
+    <col min="16" max="16" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="25">
+    <row r="1" spans="1:20" ht="25">
       <c r="A1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>26</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:20">
       <c r="C2" s="4" t="s">
         <v>0</v>
       </c>
@@ -2428,29 +2737,35 @@
       <c r="E2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="F2" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="K2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="L2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="M2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="N2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="R2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="S2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="T2" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:20">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -2466,14 +2781,14 @@
       <c r="E3" s="5">
         <v>1E-3</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="F3" s="14">
+        <v>0.182</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="I3" s="5">
-        <v>1E-3</v>
+      <c r="I3" s="4" t="s">
+        <v>3</v>
       </c>
       <c r="J3" s="5">
         <v>1E-3</v>
@@ -2484,23 +2799,29 @@
       <c r="L3" s="5">
         <v>1E-3</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="M3" s="5">
+        <v>1E-3</v>
+      </c>
+      <c r="N3" s="14">
+        <v>0.04</v>
+      </c>
+      <c r="P3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="O3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="P3" s="5">
-        <v>1E-3</v>
-      </c>
-      <c r="Q3" s="5">
-        <v>1E-3</v>
+      <c r="Q3" s="4" t="s">
+        <v>3</v>
       </c>
       <c r="R3" s="5">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="4" spans="1:18">
+      <c r="S3" s="5">
+        <v>1E-3</v>
+      </c>
+      <c r="T3" s="5">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20">
       <c r="A4" s="2"/>
       <c r="B4" s="4" t="s">
         <v>4</v>
@@ -2514,37 +2835,43 @@
       <c r="E4" s="5">
         <v>0.23951</v>
       </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="4" t="s">
+      <c r="F4" s="5">
+        <v>4.3380000000000002E-2</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="5">
+      <c r="J4" s="5">
         <v>0.30521999999999999</v>
       </c>
-      <c r="J4" s="5">
+      <c r="K4" s="5">
         <v>0.28845999999999999</v>
       </c>
-      <c r="K4" s="5">
+      <c r="L4" s="5">
         <v>0.41303000000000001</v>
       </c>
-      <c r="L4" s="5">
+      <c r="M4" s="5">
         <v>0.17415</v>
       </c>
-      <c r="N4" s="2"/>
-      <c r="O4" s="4" t="s">
+      <c r="N4" s="14">
+        <v>9.6310000000000007E-2</v>
+      </c>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="P4" s="5">
+      <c r="R4" s="5">
         <v>3.9750000000000001E-2</v>
       </c>
-      <c r="Q4" s="5">
+      <c r="S4" s="5">
         <v>0.17221</v>
       </c>
-      <c r="R4" s="5">
+      <c r="T4" s="5">
         <v>9.7350000000000006E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:20">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -2560,41 +2887,47 @@
       <c r="E5" s="5">
         <v>0.14099999999999999</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="F5" s="14">
+        <v>0.17</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="I5" s="5">
+      <c r="I5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J5" s="5">
         <v>0.20699999999999999</v>
       </c>
-      <c r="J5" s="5">
+      <c r="K5" s="5">
         <v>8.4000000000000005E-2</v>
       </c>
-      <c r="K5" s="5">
+      <c r="L5" s="5">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="L5" s="5">
+      <c r="M5" s="5">
         <v>0.75600000000000001</v>
       </c>
-      <c r="N5" s="1" t="s">
+      <c r="N5" s="14">
+        <v>0.55400000000000005</v>
+      </c>
+      <c r="P5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="O5" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="P5" s="5">
-        <v>1E-3</v>
-      </c>
-      <c r="Q5" s="5">
-        <v>1E-3</v>
+      <c r="Q5" s="4" t="s">
+        <v>3</v>
       </c>
       <c r="R5" s="5">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="6" spans="1:18">
+      <c r="S5" s="5">
+        <v>1E-3</v>
+      </c>
+      <c r="T5" s="5">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20">
       <c r="A6" s="3"/>
       <c r="B6" s="4" t="s">
         <v>7</v>
@@ -2608,48 +2941,54 @@
       <c r="E6" s="5">
         <v>2.1412749999999998</v>
       </c>
-      <c r="G6" s="3"/>
-      <c r="H6" s="4" t="s">
+      <c r="F6" s="5">
+        <v>2.0389930000000001</v>
+      </c>
+      <c r="H6" s="3"/>
+      <c r="I6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="5">
+      <c r="J6" s="5">
         <v>1.5398210000000001</v>
       </c>
-      <c r="J6" s="5">
+      <c r="K6" s="5">
         <v>3.2716630000000002</v>
       </c>
-      <c r="K6" s="5">
+      <c r="L6" s="5">
         <v>3.4585859999999999</v>
       </c>
-      <c r="L6" s="5">
+      <c r="M6" s="5">
         <v>0.26547270000000001</v>
       </c>
-      <c r="N6" s="3"/>
-      <c r="O6" s="4" t="s">
+      <c r="N6" s="5">
+        <v>0.7612833</v>
+      </c>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="P6" s="5">
+      <c r="R6" s="5">
         <v>25.059280000000001</v>
       </c>
-      <c r="Q6" s="5">
+      <c r="S6" s="5">
         <v>26.487749999999998</v>
       </c>
-      <c r="R6" s="5">
+      <c r="T6" s="5">
         <v>15.04692</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
-      <c r="I8" s="4" t="s">
+    <row r="8" spans="1:20">
+      <c r="J8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="4" t="s">
+      <c r="K8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="K8" s="4" t="s">
+      <c r="L8" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:20">
       <c r="C9" s="4" t="s">
         <v>19</v>
       </c>
@@ -2659,32 +2998,32 @@
       <c r="E9" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H9" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="I9" s="5">
+      <c r="I9" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="J9" s="5">
         <v>0.189</v>
       </c>
-      <c r="J9" s="5">
-        <v>1E-3</v>
-      </c>
       <c r="K9" s="5">
         <v>1E-3</v>
       </c>
-      <c r="P9" s="4" t="s">
+      <c r="L9" s="5">
+        <v>1E-3</v>
+      </c>
+      <c r="R9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="Q9" s="4" t="s">
+      <c r="S9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="R9" s="4" t="s">
+      <c r="T9" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:20">
       <c r="A10" s="7" t="s">
         <v>5</v>
       </c>
@@ -2700,36 +3039,36 @@
       <c r="E10" s="5">
         <v>4.7E-2</v>
       </c>
-      <c r="G10" s="2"/>
-      <c r="H10" s="12" t="s">
+      <c r="H10" s="2"/>
+      <c r="I10" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="I10" s="5">
+      <c r="J10" s="5">
         <v>2.6929999999999999E-2</v>
       </c>
-      <c r="J10" s="5">
+      <c r="K10" s="5">
         <v>0.40018999999999999</v>
       </c>
-      <c r="K10" s="5">
+      <c r="L10" s="5">
         <v>0.37597000000000003</v>
       </c>
-      <c r="N10" s="7" t="s">
+      <c r="P10" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="O10" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="P10" s="5">
-        <v>1E-3</v>
-      </c>
-      <c r="Q10" s="5">
-        <v>1E-3</v>
+      <c r="Q10" s="13" t="s">
+        <v>3</v>
       </c>
       <c r="R10" s="5">
+        <v>1E-3</v>
+      </c>
+      <c r="S10" s="5">
+        <v>1E-3</v>
+      </c>
+      <c r="T10" s="5">
         <v>2E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:20">
       <c r="A11" s="8"/>
       <c r="B11" s="8" t="s">
         <v>4</v>
@@ -2743,36 +3082,36 @@
       <c r="E11" s="5">
         <v>0.11285000000000001</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="H11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H11" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="I11" s="5">
+      <c r="I11" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="J11" s="5">
         <v>0.501</v>
       </c>
-      <c r="J11" s="5">
+      <c r="K11" s="5">
         <v>0.245</v>
       </c>
-      <c r="K11" s="5">
+      <c r="L11" s="5">
         <v>0.06</v>
       </c>
-      <c r="N11" s="8"/>
-      <c r="O11" s="8" t="s">
+      <c r="P11" s="8"/>
+      <c r="Q11" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="P11" s="5">
+      <c r="R11" s="5">
         <v>8.5290000000000005E-2</v>
       </c>
-      <c r="Q11" s="5">
+      <c r="S11" s="5">
         <v>0.20982000000000001</v>
       </c>
-      <c r="R11" s="5">
+      <c r="T11" s="5">
         <v>2.6880000000000001E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:20">
       <c r="A12" s="9" t="s">
         <v>6</v>
       </c>
@@ -2788,36 +3127,36 @@
       <c r="E12" s="5">
         <v>0.91800000000000004</v>
       </c>
-      <c r="G12" s="3"/>
-      <c r="H12" s="12" t="s">
+      <c r="H12" s="3"/>
+      <c r="I12" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="I12" s="5">
+      <c r="J12" s="5">
         <v>0.49610359999999998</v>
       </c>
-      <c r="J12" s="5">
+      <c r="K12" s="5">
         <v>1.410866</v>
       </c>
-      <c r="K12" s="5">
+      <c r="L12" s="5">
         <v>3.5674480000000002</v>
       </c>
-      <c r="N12" s="9" t="s">
+      <c r="P12" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="O12" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="P12" s="5">
-        <v>1E-3</v>
-      </c>
-      <c r="Q12" s="5">
+      <c r="Q12" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="R12" s="5">
+        <v>1E-3</v>
+      </c>
+      <c r="S12" s="5">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="R12" s="5">
+      <c r="T12" s="5">
         <v>6.5000000000000002E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:20">
       <c r="A13" s="10"/>
       <c r="B13" s="8" t="s">
         <v>7</v>
@@ -2831,283 +3170,331 @@
       <c r="E13" s="5">
         <v>1.387363E-2</v>
       </c>
-      <c r="N13" s="10"/>
-      <c r="O13" s="8" t="s">
+      <c r="P13" s="10"/>
+      <c r="Q13" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="P13" s="5">
+      <c r="R13" s="5">
         <v>30.347100000000001</v>
       </c>
-      <c r="Q13" s="5">
+      <c r="S13" s="5">
         <v>5.2194330000000004</v>
       </c>
-      <c r="R13" s="5">
+      <c r="T13" s="5">
         <v>4.0408119999999998</v>
       </c>
     </row>
-    <row r="14" spans="1:18">
-      <c r="I14" s="4" t="s">
+    <row r="14" spans="1:20">
+      <c r="J14" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="J14" s="4" t="s">
+      <c r="K14" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="K14" s="4" t="s">
+      <c r="L14" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:20">
       <c r="A15" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B15" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="H15" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I15" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="J15" s="5">
+        <v>1E-3</v>
+      </c>
+      <c r="K15" s="5">
+        <v>1E-3</v>
+      </c>
+      <c r="L15" s="5">
+        <v>1E-3</v>
+      </c>
+      <c r="P15" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q15" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="R15" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="S15" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G15" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="H15" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="I15" s="5">
-        <v>1E-3</v>
-      </c>
-      <c r="J15" s="5">
-        <v>1E-3</v>
-      </c>
-      <c r="K15" s="5">
-        <v>1E-3</v>
-      </c>
-      <c r="N15" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="O15" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="P15" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q15" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18">
+    </row>
+    <row r="16" spans="1:20">
       <c r="A16" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="5">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="C16" s="5">
-        <v>1E-3</v>
-      </c>
-      <c r="D16" s="5">
-        <v>1E-3</v>
-      </c>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8" t="s">
+      <c r="B16" s="19">
+        <v>1E-3</v>
+      </c>
+      <c r="C16" s="19">
+        <v>1E-3</v>
+      </c>
+      <c r="D16" s="19">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="E16" s="19">
+        <v>0.01</v>
+      </c>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="I16" s="5">
+      <c r="J16" s="5">
         <v>0.20022000000000001</v>
       </c>
-      <c r="J16" s="5">
+      <c r="K16" s="5">
         <v>0.37385000000000002</v>
       </c>
-      <c r="K16" s="5">
+      <c r="L16" s="5">
         <v>0.51092000000000004</v>
       </c>
-      <c r="N16" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="O16" s="5">
-        <v>1E-3</v>
-      </c>
-      <c r="P16" s="5">
-        <v>1E-3</v>
+      <c r="P16" s="4" t="s">
+        <v>3</v>
       </c>
       <c r="Q16" s="5">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="17" spans="1:17">
+      <c r="R16" s="5">
+        <v>1E-3</v>
+      </c>
+      <c r="S16" s="5">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19">
       <c r="A17" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="5">
-        <v>3.4110000000000001E-2</v>
-      </c>
-      <c r="C17" s="5">
+      <c r="B17" s="19">
         <v>0.34359000000000001</v>
       </c>
-      <c r="D17" s="14">
+      <c r="C17" s="19">
         <v>0.24163999999999999</v>
       </c>
-      <c r="G17" s="9" t="s">
+      <c r="D17" s="19">
+        <v>4.4920000000000002E-2</v>
+      </c>
+      <c r="E17" s="19">
+        <v>3.424E-2</v>
+      </c>
+      <c r="H17" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H17" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="I17" s="5">
+      <c r="I17" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="J17" s="5">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="J17" s="5">
+      <c r="K17" s="5">
         <v>0.21199999999999999</v>
       </c>
-      <c r="K17" s="5">
+      <c r="L17" s="5">
         <v>0.43</v>
       </c>
-      <c r="N17" s="4" t="s">
+      <c r="P17" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="O17" s="5">
+      <c r="Q17" s="5">
         <v>4.0039999999999999E-2</v>
       </c>
-      <c r="P17" s="14">
+      <c r="R17" s="14">
         <v>0.17221</v>
       </c>
-      <c r="Q17" s="14">
+      <c r="S17" s="14">
         <v>9.7350000000000006E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:17">
-      <c r="G18" s="10"/>
-      <c r="H18" s="8" t="s">
+    <row r="18" spans="1:19">
+      <c r="H18" s="10"/>
+      <c r="I18" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I18" s="5">
+      <c r="J18" s="5">
         <v>6.2977869999999996</v>
       </c>
-      <c r="J18" s="5">
+      <c r="K18" s="5">
         <v>1.47037</v>
       </c>
-      <c r="K18" s="5">
+      <c r="L18" s="5">
         <v>0.59589340000000002</v>
       </c>
     </row>
-    <row r="20" spans="1:17">
-      <c r="I20" s="4" t="s">
+    <row r="20" spans="1:19">
+      <c r="B20" s="15"/>
+      <c r="J20" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="J20" s="4" t="s">
+      <c r="K20" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="K20" s="4" t="s">
+      <c r="L20" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:17">
-      <c r="G21" s="7" t="s">
+    <row r="21" spans="1:19">
+      <c r="B21" s="24"/>
+      <c r="H21" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H21" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="I21" s="5">
-        <v>1E-3</v>
+      <c r="I21" s="13" t="s">
+        <v>3</v>
       </c>
       <c r="J21" s="5">
         <v>1E-3</v>
       </c>
       <c r="K21" s="5">
+        <v>1E-3</v>
+      </c>
+      <c r="L21" s="5">
         <v>4.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:17">
-      <c r="G22" s="8"/>
-      <c r="H22" s="8" t="s">
+    <row r="22" spans="1:19">
+      <c r="B22" s="24"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="I22" s="5">
+      <c r="J22" s="5">
         <v>0.18032000000000001</v>
       </c>
-      <c r="J22" s="5">
+      <c r="K22" s="5">
         <v>0.18804000000000001</v>
       </c>
-      <c r="K22" s="5">
+      <c r="L22" s="5">
         <v>5.2089999999999997E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:17">
-      <c r="G23" s="9" t="s">
+    <row r="23" spans="1:19">
+      <c r="B23" s="24"/>
+      <c r="H23" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H23" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="I23" s="5">
+      <c r="I23" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="J23" s="5">
         <v>0.85599999999999998</v>
       </c>
-      <c r="J23" s="5">
+      <c r="K23" s="5">
         <v>0.52100000000000002</v>
       </c>
-      <c r="K23" s="5">
+      <c r="L23" s="5">
         <v>0.59399999999999997</v>
       </c>
     </row>
-    <row r="24" spans="1:17">
-      <c r="G24" s="10"/>
-      <c r="H24" s="8" t="s">
+    <row r="24" spans="1:19">
+      <c r="B24" s="24"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I24" s="5">
+      <c r="J24" s="5">
         <v>2.9310409999999999E-2</v>
       </c>
-      <c r="J24" s="5">
+      <c r="K24" s="5">
         <v>0.43681009999999998</v>
       </c>
-      <c r="K24" s="5">
+      <c r="L24" s="5">
         <v>0.29608109999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:17">
-      <c r="G26" s="4" t="s">
+    <row r="25" spans="1:19">
+      <c r="B25" s="24"/>
+    </row>
+    <row r="26" spans="1:19">
+      <c r="B26" s="24"/>
+      <c r="H26" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H26" s="11" t="s">
+      <c r="I26" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="J26" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="K26" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="L26" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="M26" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="I26" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="J26" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17">
-      <c r="G27" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="H27" s="5">
-        <v>1E-3</v>
-      </c>
-      <c r="I27" s="5">
-        <v>1E-3</v>
-      </c>
-      <c r="J27" s="5">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17">
-      <c r="G28" s="4" t="s">
+    </row>
+    <row r="27" spans="1:19">
+      <c r="B27" s="24"/>
+      <c r="H27" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I27" s="19">
+        <v>1E-3</v>
+      </c>
+      <c r="J27" s="19">
+        <v>1E-3</v>
+      </c>
+      <c r="K27" s="19">
+        <v>1E-3</v>
+      </c>
+      <c r="L27" s="19">
+        <v>1E-3</v>
+      </c>
+      <c r="M27" s="19">
+        <v>1.0999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19">
+      <c r="B28" s="24"/>
+      <c r="H28" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H28" s="5">
-        <v>0.30521999999999999</v>
-      </c>
-      <c r="I28" s="14">
+      <c r="I28" s="19">
+        <v>0.28845999999999999</v>
+      </c>
+      <c r="J28" s="19">
         <v>0.12457</v>
       </c>
-      <c r="J28" s="14">
-        <v>0.17341000000000001</v>
-      </c>
+      <c r="K28" s="19">
+        <v>0.17319000000000001</v>
+      </c>
+      <c r="L28" s="19">
+        <v>7.6509999999999995E-2</v>
+      </c>
+      <c r="M28" s="19">
+        <v>0.16839999999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19">
+      <c r="B29" s="24"/>
+    </row>
+    <row r="30" spans="1:19">
+      <c r="B30" s="24"/>
+      <c r="H30" s="17"/>
+    </row>
+    <row r="31" spans="1:19">
+      <c r="B31" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3118,4 +3505,327 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="3" max="3" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="C1" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="21"/>
+      <c r="E1" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="21"/>
+      <c r="G1" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="21"/>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="C2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="19">
+        <v>1E-3</v>
+      </c>
+      <c r="F3" s="19">
+        <v>1E-3</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="23"/>
+      <c r="B4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="19">
+        <v>0.28632999999999997</v>
+      </c>
+      <c r="F4" s="19">
+        <v>0.28845999999999999</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="19">
+        <v>1E-3</v>
+      </c>
+      <c r="D5" s="19">
+        <v>1E-3</v>
+      </c>
+      <c r="E5" s="19">
+        <v>1E-3</v>
+      </c>
+      <c r="F5" s="19">
+        <v>1E-3</v>
+      </c>
+      <c r="G5" s="19">
+        <v>1E-3</v>
+      </c>
+      <c r="H5" s="19">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="23"/>
+      <c r="B6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="19">
+        <v>0.17341000000000001</v>
+      </c>
+      <c r="D6" s="19">
+        <v>0.34359000000000001</v>
+      </c>
+      <c r="E6" s="19">
+        <v>0.12687000000000001</v>
+      </c>
+      <c r="F6" s="19">
+        <v>0.12457</v>
+      </c>
+      <c r="G6" s="19">
+        <v>0.11226</v>
+      </c>
+      <c r="H6" s="19">
+        <v>0.17221</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="19">
+        <v>1E-3</v>
+      </c>
+      <c r="D7" s="19">
+        <v>1E-3</v>
+      </c>
+      <c r="E7" s="19">
+        <v>1E-3</v>
+      </c>
+      <c r="F7" s="19">
+        <v>1E-3</v>
+      </c>
+      <c r="G7" s="19">
+        <v>1E-3</v>
+      </c>
+      <c r="H7" s="19">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="23"/>
+      <c r="B8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="19">
+        <v>0.43275000000000002</v>
+      </c>
+      <c r="D8" s="19">
+        <v>0.24163999999999999</v>
+      </c>
+      <c r="E8" s="19">
+        <v>0.21772</v>
+      </c>
+      <c r="F8" s="19">
+        <v>0.17319000000000001</v>
+      </c>
+      <c r="G8" s="19">
+        <v>7.7229999999999993E-2</v>
+      </c>
+      <c r="H8" s="19">
+        <v>9.7350000000000006E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="19">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="D9" s="19">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="E9" s="19">
+        <v>1E-3</v>
+      </c>
+      <c r="F9" s="19">
+        <v>1E-3</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="23"/>
+      <c r="B10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="19">
+        <v>3.4549999999999997E-2</v>
+      </c>
+      <c r="D10" s="19">
+        <v>4.4920000000000002E-2</v>
+      </c>
+      <c r="E10" s="19">
+        <v>6.93E-2</v>
+      </c>
+      <c r="F10" s="19">
+        <v>7.6509999999999995E-2</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="19">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="D11" s="19">
+        <v>0.01</v>
+      </c>
+      <c r="E11" s="19">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="F11" s="19">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="G11" s="5">
+        <v>1E-3</v>
+      </c>
+      <c r="H11" s="5">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="23"/>
+      <c r="B12" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="19">
+        <v>4.5089999999999998E-2</v>
+      </c>
+      <c r="D12" s="19">
+        <v>3.424E-2</v>
+      </c>
+      <c r="E12" s="19">
+        <v>1.2869999999999999E-2</v>
+      </c>
+      <c r="F12" s="19">
+        <v>0.16839999999999999</v>
+      </c>
+      <c r="G12" s="5">
+        <v>3.5319999999999997E-2</v>
+      </c>
+      <c r="H12" s="5">
+        <v>4.0039999999999999E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A8"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added inland station (inland lakes)
</commit_message>
<xml_diff>
--- a/analysis/permanova_results.xlsx
+++ b/analysis/permanova_results.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="61">
   <si>
     <t>Depth</t>
   </si>
@@ -199,6 +199,12 @@
   </si>
   <si>
     <t>Residuals</t>
+  </si>
+  <si>
+    <t>0.271 (0.001***)</t>
+  </si>
+  <si>
+    <t>0.210 (0.001***)</t>
   </si>
 </sst>
 </file>
@@ -370,8 +376,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="191">
+  <cellStyleXfs count="199">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -589,12 +603,6 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -603,8 +611,14 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="191">
+  <cellStyles count="199">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -700,6 +714,10 @@
     <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -795,6 +813,10 @@
     <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3652,7 +3674,7 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="A1:G8"/>
+      <selection activeCell="G8" sqref="F8:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3666,18 +3688,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="23" t="s">
+      <c r="C1" s="28"/>
+      <c r="D1" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="24"/>
-      <c r="F1" s="23" t="s">
+      <c r="E1" s="28"/>
+      <c r="F1" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="24"/>
+      <c r="G1" s="28"/>
     </row>
     <row r="2" spans="1:10">
       <c r="B2" s="4" t="s">
@@ -3785,10 +3807,10 @@
         <v>47</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>29</v>
+        <v>60</v>
       </c>
       <c r="J6" s="22"/>
     </row>
@@ -3796,46 +3818,46 @@
       <c r="A7" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="D7" s="25" t="s">
+      <c r="D7" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="E7" s="25" t="s">
+      <c r="E7" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="F7" s="26" t="s">
+      <c r="F7" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="G7" s="26" t="s">
+      <c r="G7" s="24" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="B8" s="28">
+      <c r="B8" s="26">
         <v>0.31419999999999998</v>
       </c>
-      <c r="C8" s="28">
+      <c r="C8" s="26">
         <v>0.33561999999999997</v>
       </c>
-      <c r="D8" s="28">
+      <c r="D8" s="26">
         <v>0.28691</v>
       </c>
-      <c r="E8" s="28">
+      <c r="E8" s="26">
         <v>0.32042999999999999</v>
       </c>
-      <c r="F8" s="28">
-        <v>0.77519000000000005</v>
-      </c>
-      <c r="G8" s="28">
-        <v>0.69040000000000001</v>
+      <c r="F8" s="26">
+        <v>0.50380000000000003</v>
+      </c>
+      <c r="G8" s="26">
+        <v>0.48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated PCoA & PERMANOVA
</commit_message>
<xml_diff>
--- a/analysis/permanova_results.xlsx
+++ b/analysis/permanova_results.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="60">
   <si>
     <t>Depth</t>
   </si>
@@ -192,12 +192,6 @@
     <t>0.168 (0.011*)</t>
   </si>
   <si>
-    <t>0.040 (0.001***)</t>
-  </si>
-  <si>
-    <t>0.035 (0.001***)</t>
-  </si>
-  <si>
     <t>Residuals</t>
   </si>
   <si>
@@ -205,6 +199,9 @@
   </si>
   <si>
     <t>0.210 (0.001***)</t>
+  </si>
+  <si>
+    <t>0.095 (0.001***)</t>
   </si>
 </sst>
 </file>
@@ -3674,7 +3671,7 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="F8:G8"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3807,10 +3804,10 @@
         <v>47</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J6" s="22"/>
     </row>
@@ -3831,15 +3828,15 @@
         <v>55</v>
       </c>
       <c r="F7" s="24" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="G7" s="24" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="25" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B8" s="26">
         <v>0.31419999999999998</v>
@@ -3854,10 +3851,10 @@
         <v>0.32042999999999999</v>
       </c>
       <c r="F8" s="26">
-        <v>0.50380000000000003</v>
+        <v>0.46100000000000002</v>
       </c>
       <c r="G8" s="26">
-        <v>0.48</v>
+        <v>0.42499999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>